<commit_message>
my survey final ver 1
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="762">
   <si>
     <t>code</t>
   </si>
@@ -2308,6 +2308,9 @@
   </si>
   <si>
     <t>ELT2038 1</t>
+  </si>
+  <si>
+    <t>course_id</t>
   </si>
 </sst>
 </file>
@@ -2382,7 +2385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2402,6 +2405,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2682,22 +2688,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E288"/>
+  <dimension ref="A1:F288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F1" sqref="F1:F288"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2713,8 +2720,11 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2730,8 +2740,11 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -2747,8 +2760,11 @@
       <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -2764,8 +2780,11 @@
       <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -2781,8 +2800,11 @@
       <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -2798,8 +2820,11 @@
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -2815,8 +2840,11 @@
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -2832,8 +2860,11 @@
       <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -2849,8 +2880,11 @@
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -2866,8 +2900,11 @@
       <c r="E10" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -2883,8 +2920,11 @@
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -2900,8 +2940,11 @@
       <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -2917,8 +2960,11 @@
       <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -2934,8 +2980,11 @@
       <c r="E14" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
@@ -2951,8 +3000,11 @@
       <c r="E15" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
@@ -2968,8 +3020,11 @@
       <c r="E16" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -2985,8 +3040,11 @@
       <c r="E17" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -3002,8 +3060,11 @@
       <c r="E18" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>57</v>
       </c>
@@ -3019,8 +3080,11 @@
       <c r="E19" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -3036,8 +3100,11 @@
       <c r="E20" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>57</v>
       </c>
@@ -3053,8 +3120,11 @@
       <c r="E21" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>64</v>
       </c>
@@ -3070,8 +3140,11 @@
       <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>68</v>
       </c>
@@ -3087,8 +3160,11 @@
       <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>68</v>
       </c>
@@ -3104,8 +3180,11 @@
       <c r="E24" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>73</v>
       </c>
@@ -3121,8 +3200,11 @@
       <c r="E25" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>73</v>
       </c>
@@ -3138,8 +3220,11 @@
       <c r="E26" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>78</v>
       </c>
@@ -3155,8 +3240,11 @@
       <c r="E27" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>81</v>
       </c>
@@ -3172,8 +3260,11 @@
       <c r="E28" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>84</v>
       </c>
@@ -3189,8 +3280,11 @@
       <c r="E29" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>84</v>
       </c>
@@ -3206,8 +3300,11 @@
       <c r="E30" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>89</v>
       </c>
@@ -3223,8 +3320,11 @@
       <c r="E31" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>92</v>
       </c>
@@ -3240,8 +3340,11 @@
       <c r="E32" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>92</v>
       </c>
@@ -3257,8 +3360,11 @@
       <c r="E33" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>96</v>
       </c>
@@ -3274,8 +3380,11 @@
       <c r="E34" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>96</v>
       </c>
@@ -3291,8 +3400,11 @@
       <c r="E35" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>99</v>
       </c>
@@ -3308,8 +3420,11 @@
       <c r="E36" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>101</v>
       </c>
@@ -3325,8 +3440,11 @@
       <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>104</v>
       </c>
@@ -3342,8 +3460,11 @@
       <c r="E38" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>107</v>
       </c>
@@ -3359,8 +3480,11 @@
       <c r="E39" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>110</v>
       </c>
@@ -3376,8 +3500,11 @@
       <c r="E40" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>113</v>
       </c>
@@ -3393,8 +3520,11 @@
       <c r="E41" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>116</v>
       </c>
@@ -3410,8 +3540,11 @@
       <c r="E42" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>116</v>
       </c>
@@ -3427,8 +3560,11 @@
       <c r="E43" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>116</v>
       </c>
@@ -3444,8 +3580,11 @@
       <c r="E44" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>116</v>
       </c>
@@ -3461,8 +3600,11 @@
       <c r="E45" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>122</v>
       </c>
@@ -3478,8 +3620,11 @@
       <c r="E46" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>125</v>
       </c>
@@ -3495,8 +3640,11 @@
       <c r="E47" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>129</v>
       </c>
@@ -3512,8 +3660,11 @@
       <c r="E48" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>133</v>
       </c>
@@ -3529,8 +3680,11 @@
       <c r="E49" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>133</v>
       </c>
@@ -3546,8 +3700,11 @@
       <c r="E50" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>140</v>
       </c>
@@ -3563,8 +3720,11 @@
       <c r="E51" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>144</v>
       </c>
@@ -3580,8 +3740,11 @@
       <c r="E52" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F52" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>148</v>
       </c>
@@ -3597,8 +3760,11 @@
       <c r="E53" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>148</v>
       </c>
@@ -3614,8 +3780,11 @@
       <c r="E54" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>153</v>
       </c>
@@ -3631,8 +3800,11 @@
       <c r="E55" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>153</v>
       </c>
@@ -3648,8 +3820,11 @@
       <c r="E56" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>158</v>
       </c>
@@ -3665,8 +3840,11 @@
       <c r="E57" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F57" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>158</v>
       </c>
@@ -3682,8 +3860,11 @@
       <c r="E58" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>163</v>
       </c>
@@ -3699,8 +3880,11 @@
       <c r="E59" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F59" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>166</v>
       </c>
@@ -3716,8 +3900,11 @@
       <c r="E60" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>166</v>
       </c>
@@ -3733,8 +3920,11 @@
       <c r="E61" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>171</v>
       </c>
@@ -3750,8 +3940,11 @@
       <c r="E62" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>175</v>
       </c>
@@ -3767,8 +3960,11 @@
       <c r="E63" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F63" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>175</v>
       </c>
@@ -3784,8 +3980,11 @@
       <c r="E64" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F64" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>180</v>
       </c>
@@ -3801,8 +4000,11 @@
       <c r="E65" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F65" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>184</v>
       </c>
@@ -3818,8 +4020,11 @@
       <c r="E66" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F66" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>184</v>
       </c>
@@ -3835,8 +4040,11 @@
       <c r="E67" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F67" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>188</v>
       </c>
@@ -3852,8 +4060,11 @@
       <c r="E68" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F68" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>188</v>
       </c>
@@ -3869,8 +4080,11 @@
       <c r="E69" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F69" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>188</v>
       </c>
@@ -3886,8 +4100,11 @@
       <c r="E70" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F70" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>188</v>
       </c>
@@ -3903,8 +4120,11 @@
       <c r="E71" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F71" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>196</v>
       </c>
@@ -3920,8 +4140,11 @@
       <c r="E72" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F72" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>200</v>
       </c>
@@ -3937,8 +4160,11 @@
       <c r="E73" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F73" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>203</v>
       </c>
@@ -3954,8 +4180,11 @@
       <c r="E74" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F74" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>207</v>
       </c>
@@ -3971,8 +4200,11 @@
       <c r="E75" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F75" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>211</v>
       </c>
@@ -3988,8 +4220,11 @@
       <c r="E76" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F76" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>214</v>
       </c>
@@ -4005,8 +4240,11 @@
       <c r="E77" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F77" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>217</v>
       </c>
@@ -4022,8 +4260,11 @@
       <c r="E78" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F78" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>221</v>
       </c>
@@ -4039,8 +4280,11 @@
       <c r="E79" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F79" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>225</v>
       </c>
@@ -4056,8 +4300,11 @@
       <c r="E80" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F80" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>229</v>
       </c>
@@ -4073,8 +4320,11 @@
       <c r="E81" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F81" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>232</v>
       </c>
@@ -4090,8 +4340,11 @@
       <c r="E82" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F82" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>235</v>
       </c>
@@ -4107,8 +4360,11 @@
       <c r="E83" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F83" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>238</v>
       </c>
@@ -4124,8 +4380,11 @@
       <c r="E84" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F84" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>242</v>
       </c>
@@ -4141,8 +4400,11 @@
       <c r="E85" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F85" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>245</v>
       </c>
@@ -4158,8 +4420,11 @@
       <c r="E86" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F86" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>249</v>
       </c>
@@ -4175,8 +4440,11 @@
       <c r="E87" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F87" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>253</v>
       </c>
@@ -4192,8 +4460,11 @@
       <c r="E88" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F88" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>257</v>
       </c>
@@ -4209,8 +4480,11 @@
       <c r="E89" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F89" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>260</v>
       </c>
@@ -4226,8 +4500,11 @@
       <c r="E90" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F90" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>264</v>
       </c>
@@ -4243,8 +4520,11 @@
       <c r="E91" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F91" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>268</v>
       </c>
@@ -4260,8 +4540,11 @@
       <c r="E92" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F92" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>272</v>
       </c>
@@ -4277,8 +4560,11 @@
       <c r="E93" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F93" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>276</v>
       </c>
@@ -4294,8 +4580,11 @@
       <c r="E94" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F94" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>280</v>
       </c>
@@ -4311,8 +4600,11 @@
       <c r="E95" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F95" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>284</v>
       </c>
@@ -4328,8 +4620,11 @@
       <c r="E96" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F96" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>288</v>
       </c>
@@ -4345,8 +4640,11 @@
       <c r="E97" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F97" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>292</v>
       </c>
@@ -4362,8 +4660,11 @@
       <c r="E98" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F98" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>296</v>
       </c>
@@ -4379,8 +4680,11 @@
       <c r="E99" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F99" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>300</v>
       </c>
@@ -4396,8 +4700,11 @@
       <c r="E100" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F100" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>304</v>
       </c>
@@ -4413,8 +4720,11 @@
       <c r="E101" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F101" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>308</v>
       </c>
@@ -4430,8 +4740,11 @@
       <c r="E102" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F102" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>312</v>
       </c>
@@ -4447,8 +4760,11 @@
       <c r="E103" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F103" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>316</v>
       </c>
@@ -4464,8 +4780,11 @@
       <c r="E104" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F104" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>320</v>
       </c>
@@ -4481,8 +4800,11 @@
       <c r="E105" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F105" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>323</v>
       </c>
@@ -4498,8 +4820,11 @@
       <c r="E106" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F106" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>327</v>
       </c>
@@ -4515,8 +4840,11 @@
       <c r="E107" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F107" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>330</v>
       </c>
@@ -4532,8 +4860,11 @@
       <c r="E108" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F108" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>333</v>
       </c>
@@ -4549,8 +4880,11 @@
       <c r="E109" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F109" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>336</v>
       </c>
@@ -4566,8 +4900,11 @@
       <c r="E110" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F110" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>338</v>
       </c>
@@ -4583,8 +4920,11 @@
       <c r="E111" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F111" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>341</v>
       </c>
@@ -4600,8 +4940,11 @@
       <c r="E112" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F112" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>344</v>
       </c>
@@ -4617,8 +4960,11 @@
       <c r="E113" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F113" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>348</v>
       </c>
@@ -4634,8 +4980,11 @@
       <c r="E114" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F114" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>351</v>
       </c>
@@ -4651,8 +5000,11 @@
       <c r="E115" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F115" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>355</v>
       </c>
@@ -4668,8 +5020,11 @@
       <c r="E116" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F116" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>359</v>
       </c>
@@ -4685,8 +5040,11 @@
       <c r="E117" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F117" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>363</v>
       </c>
@@ -4702,8 +5060,11 @@
       <c r="E118" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F118" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>365</v>
       </c>
@@ -4719,8 +5080,11 @@
       <c r="E119" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F119" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>369</v>
       </c>
@@ -4736,8 +5100,11 @@
       <c r="E120" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F120" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>373</v>
       </c>
@@ -4753,8 +5120,11 @@
       <c r="E121" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F121" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>376</v>
       </c>
@@ -4770,8 +5140,11 @@
       <c r="E122" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F122" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>380</v>
       </c>
@@ -4787,8 +5160,11 @@
       <c r="E123" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F123" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>384</v>
       </c>
@@ -4804,8 +5180,11 @@
       <c r="E124" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F124" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>388</v>
       </c>
@@ -4821,8 +5200,11 @@
       <c r="E125" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F125" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>390</v>
       </c>
@@ -4838,8 +5220,11 @@
       <c r="E126" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F126" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>394</v>
       </c>
@@ -4855,8 +5240,11 @@
       <c r="E127" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F127" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>398</v>
       </c>
@@ -4872,8 +5260,11 @@
       <c r="E128" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F128" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>401</v>
       </c>
@@ -4889,8 +5280,11 @@
       <c r="E129" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F129" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>405</v>
       </c>
@@ -4906,8 +5300,11 @@
       <c r="E130" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F130" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>405</v>
       </c>
@@ -4923,8 +5320,11 @@
       <c r="E131" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F131" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>405</v>
       </c>
@@ -4940,8 +5340,11 @@
       <c r="E132" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F132" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>405</v>
       </c>
@@ -4957,8 +5360,11 @@
       <c r="E133" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F133" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>405</v>
       </c>
@@ -4974,8 +5380,11 @@
       <c r="E134" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F134" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>405</v>
       </c>
@@ -4991,8 +5400,11 @@
       <c r="E135" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F135" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>405</v>
       </c>
@@ -5008,8 +5420,11 @@
       <c r="E136" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F136" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>405</v>
       </c>
@@ -5025,8 +5440,11 @@
       <c r="E137" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F137" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>405</v>
       </c>
@@ -5042,8 +5460,11 @@
       <c r="E138" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F138" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>405</v>
       </c>
@@ -5059,8 +5480,11 @@
       <c r="E139" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F139" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>405</v>
       </c>
@@ -5076,8 +5500,11 @@
       <c r="E140" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F140" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>405</v>
       </c>
@@ -5093,8 +5520,11 @@
       <c r="E141" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F141" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>428</v>
       </c>
@@ -5110,8 +5540,11 @@
       <c r="E142" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F142" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>428</v>
       </c>
@@ -5127,8 +5560,11 @@
       <c r="E143" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F143" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>428</v>
       </c>
@@ -5144,8 +5580,11 @@
       <c r="E144" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F144" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>433</v>
       </c>
@@ -5161,8 +5600,11 @@
       <c r="E145" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F145" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>433</v>
       </c>
@@ -5178,8 +5620,11 @@
       <c r="E146" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F146" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>433</v>
       </c>
@@ -5195,8 +5640,11 @@
       <c r="E147" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F147" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>433</v>
       </c>
@@ -5212,8 +5660,11 @@
       <c r="E148" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F148" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>433</v>
       </c>
@@ -5229,8 +5680,11 @@
       <c r="E149" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F149" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>433</v>
       </c>
@@ -5246,8 +5700,11 @@
       <c r="E150" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F150" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>433</v>
       </c>
@@ -5263,8 +5720,11 @@
       <c r="E151" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F151" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>433</v>
       </c>
@@ -5280,8 +5740,11 @@
       <c r="E152" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F152" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>433</v>
       </c>
@@ -5297,8 +5760,11 @@
       <c r="E153" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F153" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>451</v>
       </c>
@@ -5314,8 +5780,11 @@
       <c r="E154" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F154" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>451</v>
       </c>
@@ -5331,8 +5800,11 @@
       <c r="E155" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F155" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>451</v>
       </c>
@@ -5348,8 +5820,11 @@
       <c r="E156" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F156" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>459</v>
       </c>
@@ -5365,8 +5840,11 @@
       <c r="E157" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F157" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>463</v>
       </c>
@@ -5382,8 +5860,11 @@
       <c r="E158" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F158" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>465</v>
       </c>
@@ -5399,8 +5880,11 @@
       <c r="E159" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F159" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>468</v>
       </c>
@@ -5416,8 +5900,11 @@
       <c r="E160" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F160" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>468</v>
       </c>
@@ -5433,8 +5920,11 @@
       <c r="E161" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F161" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>473</v>
       </c>
@@ -5450,8 +5940,11 @@
       <c r="E162" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F162" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>473</v>
       </c>
@@ -5467,8 +5960,11 @@
       <c r="E163" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F163" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>473</v>
       </c>
@@ -5484,8 +5980,11 @@
       <c r="E164" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F164" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>480</v>
       </c>
@@ -5501,8 +6000,11 @@
       <c r="E165" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F165" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>480</v>
       </c>
@@ -5518,8 +6020,11 @@
       <c r="E166" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F166" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>480</v>
       </c>
@@ -5535,8 +6040,11 @@
       <c r="E167" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F167" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>480</v>
       </c>
@@ -5552,8 +6060,11 @@
       <c r="E168" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F168" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>480</v>
       </c>
@@ -5569,8 +6080,11 @@
       <c r="E169" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F169" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>480</v>
       </c>
@@ -5586,8 +6100,11 @@
       <c r="E170" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F170" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>493</v>
       </c>
@@ -5603,8 +6120,11 @@
       <c r="E171" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F171" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>493</v>
       </c>
@@ -5620,8 +6140,11 @@
       <c r="E172" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F172" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>493</v>
       </c>
@@ -5637,8 +6160,11 @@
       <c r="E173" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F173" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>493</v>
       </c>
@@ -5654,8 +6180,11 @@
       <c r="E174" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F174" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>493</v>
       </c>
@@ -5671,8 +6200,11 @@
       <c r="E175" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F175" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>493</v>
       </c>
@@ -5688,8 +6220,11 @@
       <c r="E176" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F176" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>505</v>
       </c>
@@ -5705,8 +6240,11 @@
       <c r="E177" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F177" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>505</v>
       </c>
@@ -5722,8 +6260,11 @@
       <c r="E178" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F178" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>505</v>
       </c>
@@ -5739,8 +6280,11 @@
       <c r="E179" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F179" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>505</v>
       </c>
@@ -5756,8 +6300,11 @@
       <c r="E180" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F180" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>505</v>
       </c>
@@ -5773,8 +6320,11 @@
       <c r="E181" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F181" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>514</v>
       </c>
@@ -5790,8 +6340,11 @@
       <c r="E182" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F182" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>518</v>
       </c>
@@ -5807,8 +6360,11 @@
       <c r="E183" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F183" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>521</v>
       </c>
@@ -5824,8 +6380,11 @@
       <c r="E184" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F184" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>525</v>
       </c>
@@ -5841,8 +6400,11 @@
       <c r="E185" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F185" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>529</v>
       </c>
@@ -5858,8 +6420,11 @@
       <c r="E186" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F186" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>533</v>
       </c>
@@ -5875,8 +6440,11 @@
       <c r="E187" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F187" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>536</v>
       </c>
@@ -5892,8 +6460,11 @@
       <c r="E188" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F188" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>540</v>
       </c>
@@ -5909,8 +6480,11 @@
       <c r="E189" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F189" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>544</v>
       </c>
@@ -5926,8 +6500,11 @@
       <c r="E190" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F190" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>544</v>
       </c>
@@ -5943,8 +6520,11 @@
       <c r="E191" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F191" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>550</v>
       </c>
@@ -5960,8 +6540,11 @@
       <c r="E192" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F192" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>554</v>
       </c>
@@ -5977,8 +6560,11 @@
       <c r="E193" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F193" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>557</v>
       </c>
@@ -5994,8 +6580,11 @@
       <c r="E194" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F194" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>560</v>
       </c>
@@ -6011,8 +6600,11 @@
       <c r="E195" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F195" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>564</v>
       </c>
@@ -6028,8 +6620,11 @@
       <c r="E196" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F196" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>567</v>
       </c>
@@ -6045,8 +6640,11 @@
       <c r="E197" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F197" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>571</v>
       </c>
@@ -6062,8 +6660,11 @@
       <c r="E198" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F198" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>575</v>
       </c>
@@ -6079,8 +6680,11 @@
       <c r="E199" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F199" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>575</v>
       </c>
@@ -6096,8 +6700,11 @@
       <c r="E200" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F200" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>575</v>
       </c>
@@ -6113,8 +6720,11 @@
       <c r="E201" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F201" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>575</v>
       </c>
@@ -6130,8 +6740,11 @@
       <c r="E202" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F202" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>575</v>
       </c>
@@ -6147,8 +6760,11 @@
       <c r="E203" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F203" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>585</v>
       </c>
@@ -6164,8 +6780,11 @@
       <c r="E204" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F204" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>585</v>
       </c>
@@ -6181,8 +6800,11 @@
       <c r="E205" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F205" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>589</v>
       </c>
@@ -6198,8 +6820,11 @@
       <c r="E206" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F206" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>592</v>
       </c>
@@ -6215,8 +6840,11 @@
       <c r="E207" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F207" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>595</v>
       </c>
@@ -6232,8 +6860,11 @@
       <c r="E208" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F208" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>595</v>
       </c>
@@ -6249,8 +6880,11 @@
       <c r="E209" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F209" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
         <v>602</v>
       </c>
@@ -6266,8 +6900,11 @@
       <c r="E210" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F210" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>605</v>
       </c>
@@ -6283,8 +6920,11 @@
       <c r="E211" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F211" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>605</v>
       </c>
@@ -6300,8 +6940,11 @@
       <c r="E212" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F212" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>608</v>
       </c>
@@ -6317,8 +6960,11 @@
       <c r="E213" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F213" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>608</v>
       </c>
@@ -6334,8 +6980,11 @@
       <c r="E214" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F214" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>608</v>
       </c>
@@ -6351,8 +7000,11 @@
       <c r="E215" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F215" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>608</v>
       </c>
@@ -6368,8 +7020,11 @@
       <c r="E216" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F216" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>616</v>
       </c>
@@ -6385,8 +7040,11 @@
       <c r="E217" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F217" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
         <v>620</v>
       </c>
@@ -6402,8 +7060,11 @@
       <c r="E218" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F218" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>624</v>
       </c>
@@ -6419,8 +7080,11 @@
       <c r="E219" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F219" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>627</v>
       </c>
@@ -6436,8 +7100,11 @@
       <c r="E220" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F220" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>627</v>
       </c>
@@ -6453,8 +7120,11 @@
       <c r="E221" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F221" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>631</v>
       </c>
@@ -6470,8 +7140,11 @@
       <c r="E222" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F222" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>635</v>
       </c>
@@ -6487,8 +7160,11 @@
       <c r="E223" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F223" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>638</v>
       </c>
@@ -6504,8 +7180,11 @@
       <c r="E224" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F224" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>641</v>
       </c>
@@ -6521,8 +7200,11 @@
       <c r="E225" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F225" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>641</v>
       </c>
@@ -6538,8 +7220,11 @@
       <c r="E226" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F226" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>641</v>
       </c>
@@ -6555,8 +7240,11 @@
       <c r="E227" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F227" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>641</v>
       </c>
@@ -6572,8 +7260,11 @@
       <c r="E228" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F228" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>641</v>
       </c>
@@ -6589,8 +7280,11 @@
       <c r="E229" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F229" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>641</v>
       </c>
@@ -6606,8 +7300,11 @@
       <c r="E230" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F230" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>641</v>
       </c>
@@ -6623,8 +7320,11 @@
       <c r="E231" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F231" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>641</v>
       </c>
@@ -6640,8 +7340,11 @@
       <c r="E232" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F232" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>641</v>
       </c>
@@ -6657,8 +7360,11 @@
       <c r="E233" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F233" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="6" t="s">
         <v>656</v>
       </c>
@@ -6674,8 +7380,11 @@
       <c r="E234" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F234" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="6" t="s">
         <v>659</v>
       </c>
@@ -6691,8 +7400,11 @@
       <c r="E235" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F235" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>662</v>
       </c>
@@ -6708,8 +7420,11 @@
       <c r="E236" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F236" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="6" t="s">
         <v>666</v>
       </c>
@@ -6725,8 +7440,11 @@
       <c r="E237" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F237" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="6" t="s">
         <v>669</v>
       </c>
@@ -6742,8 +7460,11 @@
       <c r="E238" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F238" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>672</v>
       </c>
@@ -6759,8 +7480,11 @@
       <c r="E239" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F239" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>672</v>
       </c>
@@ -6776,8 +7500,11 @@
       <c r="E240" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F240" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>672</v>
       </c>
@@ -6793,8 +7520,11 @@
       <c r="E241" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F241" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>672</v>
       </c>
@@ -6810,8 +7540,11 @@
       <c r="E242" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F242" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>672</v>
       </c>
@@ -6827,8 +7560,11 @@
       <c r="E243" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F243" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>672</v>
       </c>
@@ -6844,8 +7580,11 @@
       <c r="E244" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F244" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>672</v>
       </c>
@@ -6861,8 +7600,11 @@
       <c r="E245" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F245" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>672</v>
       </c>
@@ -6878,8 +7620,11 @@
       <c r="E246" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F246" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>686</v>
       </c>
@@ -6895,8 +7640,11 @@
       <c r="E247" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F247" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>686</v>
       </c>
@@ -6912,8 +7660,11 @@
       <c r="E248" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F248" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>686</v>
       </c>
@@ -6929,8 +7680,11 @@
       <c r="E249" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F249" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>686</v>
       </c>
@@ -6946,8 +7700,11 @@
       <c r="E250" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F250" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>686</v>
       </c>
@@ -6963,8 +7720,11 @@
       <c r="E251" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F251" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>686</v>
       </c>
@@ -6980,8 +7740,11 @@
       <c r="E252" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F252" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="5" t="s">
         <v>686</v>
       </c>
@@ -6997,8 +7760,11 @@
       <c r="E253" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F253" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="5" t="s">
         <v>686</v>
       </c>
@@ -7014,8 +7780,11 @@
       <c r="E254" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="255" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F254" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
         <v>686</v>
       </c>
@@ -7031,8 +7800,11 @@
       <c r="E255" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F255" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="5" t="s">
         <v>686</v>
       </c>
@@ -7048,8 +7820,11 @@
       <c r="E256" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F256" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="5" t="s">
         <v>686</v>
       </c>
@@ -7065,8 +7840,11 @@
       <c r="E257" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="258" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F257" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="5" t="s">
         <v>686</v>
       </c>
@@ -7082,8 +7860,11 @@
       <c r="E258" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F258" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="5" t="s">
         <v>686</v>
       </c>
@@ -7099,8 +7880,11 @@
       <c r="E259" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F259" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="5" t="s">
         <v>711</v>
       </c>
@@ -7116,8 +7900,11 @@
       <c r="E260" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="261" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F260" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="5" t="s">
         <v>711</v>
       </c>
@@ -7133,8 +7920,11 @@
       <c r="E261" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="262" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F261" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="5" t="s">
         <v>711</v>
       </c>
@@ -7150,8 +7940,11 @@
       <c r="E262" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F262" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="5" t="s">
         <v>716</v>
       </c>
@@ -7167,8 +7960,11 @@
       <c r="E263" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="264" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F263" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="5" t="s">
         <v>716</v>
       </c>
@@ -7184,8 +7980,11 @@
       <c r="E264" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="265" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F264" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="5" t="s">
         <v>720</v>
       </c>
@@ -7201,8 +8000,11 @@
       <c r="E265" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="266" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F265" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="5" t="s">
         <v>720</v>
       </c>
@@ -7218,8 +8020,11 @@
       <c r="E266" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="267" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F266" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="5" t="s">
         <v>720</v>
       </c>
@@ -7235,8 +8040,11 @@
       <c r="E267" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="268" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F267" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="5" t="s">
         <v>725</v>
       </c>
@@ -7252,8 +8060,11 @@
       <c r="E268" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="269" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F268" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="5" t="s">
         <v>725</v>
       </c>
@@ -7269,8 +8080,11 @@
       <c r="E269" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="270" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F269" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="5" t="s">
         <v>730</v>
       </c>
@@ -7286,8 +8100,11 @@
       <c r="E270" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="271" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F270" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="5" t="s">
         <v>730</v>
       </c>
@@ -7303,8 +8120,11 @@
       <c r="E271" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F271" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="5" t="s">
         <v>730</v>
       </c>
@@ -7320,8 +8140,11 @@
       <c r="E272" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="273" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F272" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="5" t="s">
         <v>730</v>
       </c>
@@ -7337,8 +8160,11 @@
       <c r="E273" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="274" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F273" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="5" t="s">
         <v>730</v>
       </c>
@@ -7354,8 +8180,11 @@
       <c r="E274" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="275" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F274" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="5" t="s">
         <v>730</v>
       </c>
@@ -7371,8 +8200,11 @@
       <c r="E275" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="276" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F275" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="5" t="s">
         <v>730</v>
       </c>
@@ -7388,8 +8220,11 @@
       <c r="E276" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F276" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="5" t="s">
         <v>730</v>
       </c>
@@ -7405,8 +8240,11 @@
       <c r="E277" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="278" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F277" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="5" t="s">
         <v>730</v>
       </c>
@@ -7422,8 +8260,11 @@
       <c r="E278" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="279" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F278" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A279" s="5" t="s">
         <v>730</v>
       </c>
@@ -7439,8 +8280,11 @@
       <c r="E279" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="280" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F279" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="5" t="s">
         <v>730</v>
       </c>
@@ -7456,8 +8300,11 @@
       <c r="E280" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="281" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F280" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="5" t="s">
         <v>730</v>
       </c>
@@ -7473,8 +8320,11 @@
       <c r="E281" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="282" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F281" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="5" t="s">
         <v>730</v>
       </c>
@@ -7490,8 +8340,11 @@
       <c r="E282" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="283" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F282" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6" t="s">
         <v>749</v>
       </c>
@@ -7507,8 +8360,11 @@
       <c r="E283" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="284" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F283" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6" t="s">
         <v>749</v>
       </c>
@@ -7524,8 +8380,11 @@
       <c r="E284" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="285" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F284" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6" t="s">
         <v>749</v>
       </c>
@@ -7541,8 +8400,11 @@
       <c r="E285" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="286" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F285" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6" t="s">
         <v>749</v>
       </c>
@@ -7558,8 +8420,11 @@
       <c r="E286" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F286" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="5" t="s">
         <v>756</v>
       </c>
@@ -7575,8 +8440,11 @@
       <c r="E287" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F287" s="9">
+        <v>17181</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="5" t="s">
         <v>756</v>
       </c>
@@ -7591,6 +8459,9 @@
       </c>
       <c r="E288" s="4" t="s">
         <v>409</v>
+      </c>
+      <c r="F288" s="9">
+        <v>17181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>